<commit_message>
Chnage mysql table column type to Date
</commit_message>
<xml_diff>
--- a/Research Performance Tracker.xlsx
+++ b/Research Performance Tracker.xlsx
@@ -1080,7 +1080,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -1826,18 +1826,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1845,8 +1862,89 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1862,9 +1960,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1890,159 +1985,22 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="12"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
 </styleSheet>
 </file>
@@ -2359,22 +2317,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="20" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
     </row>
     <row r="2" spans="1:14" s="84" customFormat="1">
       <c r="A2" s="84" t="s">
@@ -2424,30 +2382,30 @@
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="123" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="122"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="122"/>
-      <c r="H10" s="122"/>
-      <c r="I10" s="122"/>
-      <c r="J10" s="122"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="123"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="122"/>
-      <c r="B11" s="122"/>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="122"/>
-      <c r="H11" s="122"/>
-      <c r="I11" s="122"/>
-      <c r="J11" s="122"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="123"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="123"/>
+      <c r="E11" s="123"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="123"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="123"/>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="4" t="s">
@@ -2517,35 +2475,35 @@
       <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:27" ht="15.75" thickTop="1" thickBot="1">
-      <c r="A30" s="113" t="s">
+      <c r="A30" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="114"/>
-      <c r="I30" s="114"/>
-      <c r="J30" s="114"/>
-      <c r="K30" s="114"/>
-      <c r="L30" s="115"/>
-      <c r="O30" s="118" t="s">
+      <c r="B30" s="110"/>
+      <c r="C30" s="110"/>
+      <c r="D30" s="110"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="110"/>
+      <c r="G30" s="110"/>
+      <c r="H30" s="110"/>
+      <c r="I30" s="110"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="110"/>
+      <c r="L30" s="111"/>
+      <c r="O30" s="119" t="s">
         <v>87</v>
       </c>
-      <c r="P30" s="119"/>
-      <c r="Q30" s="119"/>
-      <c r="R30" s="119"/>
-      <c r="S30" s="119"/>
-      <c r="T30" s="119"/>
-      <c r="U30" s="119"/>
-      <c r="V30" s="119"/>
-      <c r="W30" s="119"/>
-      <c r="X30" s="119"/>
-      <c r="Y30" s="119"/>
-      <c r="Z30" s="119"/>
-      <c r="AA30" s="120"/>
+      <c r="P30" s="120"/>
+      <c r="Q30" s="120"/>
+      <c r="R30" s="120"/>
+      <c r="S30" s="120"/>
+      <c r="T30" s="120"/>
+      <c r="U30" s="120"/>
+      <c r="V30" s="120"/>
+      <c r="W30" s="120"/>
+      <c r="X30" s="120"/>
+      <c r="Y30" s="120"/>
+      <c r="Z30" s="120"/>
+      <c r="AA30" s="121"/>
     </row>
     <row r="31" spans="1:27" ht="15" thickTop="1">
       <c r="A31" s="5" t="s">
@@ -2616,17 +2574,17 @@
       <c r="AA33" s="39"/>
     </row>
     <row r="34" spans="1:27">
-      <c r="A34" s="123" t="s">
+      <c r="A34" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="123"/>
-      <c r="C34" s="123"/>
-      <c r="D34" s="123"/>
-      <c r="E34" s="123"/>
-      <c r="F34" s="123"/>
-      <c r="G34" s="123"/>
-      <c r="H34" s="123"/>
-      <c r="I34" s="123"/>
+      <c r="B34" s="92"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="92"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="92"/>
+      <c r="G34" s="92"/>
+      <c r="H34" s="92"/>
+      <c r="I34" s="92"/>
       <c r="O34" s="37"/>
       <c r="P34" s="38"/>
       <c r="Q34" s="38"/>
@@ -2663,9 +2621,9 @@
       <c r="G35" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K35" s="124"/>
-      <c r="L35" s="125"/>
-      <c r="M35" s="125"/>
+      <c r="K35" s="93"/>
+      <c r="L35" s="94"/>
+      <c r="M35" s="94"/>
       <c r="O35" s="37"/>
       <c r="P35" s="38"/>
       <c r="Q35" s="38"/>
@@ -2767,108 +2725,108 @@
       <c r="AA38" s="39"/>
     </row>
     <row r="39" spans="1:27" ht="45" customHeight="1">
-      <c r="A39" s="126" t="s">
+      <c r="A39" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="128" t="s">
+      <c r="B39" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="93" t="s">
+      <c r="C39" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="93" t="s">
+      <c r="D39" s="98" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="93" t="s">
+      <c r="E39" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="95" t="s">
+      <c r="F39" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="G39" s="95" t="s">
+      <c r="G39" s="124" t="s">
         <v>27</v>
       </c>
-      <c r="H39" s="95" t="s">
+      <c r="H39" s="124" t="s">
         <v>22</v>
       </c>
-      <c r="I39" s="93" t="s">
+      <c r="I39" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="J39" s="93" t="s">
+      <c r="J39" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="K39" s="93" t="s">
+      <c r="K39" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="L39" s="93" t="s">
+      <c r="L39" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="O39" s="121" t="s">
+      <c r="O39" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="P39" s="111" t="s">
+      <c r="P39" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="Q39" s="111" t="s">
+      <c r="Q39" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="R39" s="111" t="s">
+      <c r="R39" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="S39" s="111" t="s">
+      <c r="S39" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="T39" s="111" t="s">
+      <c r="T39" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="U39" s="111" t="s">
+      <c r="U39" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="V39" s="111" t="s">
+      <c r="V39" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="W39" s="111" t="s">
+      <c r="W39" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="X39" s="111" t="s">
+      <c r="X39" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="Y39" s="111" t="s">
+      <c r="Y39" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="Z39" s="111" t="s">
+      <c r="Z39" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="AA39" s="116" t="s">
+      <c r="AA39" s="117" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:27">
-      <c r="A40" s="127"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="94"/>
-      <c r="D40" s="94"/>
-      <c r="E40" s="94"/>
-      <c r="F40" s="95"/>
-      <c r="G40" s="95"/>
-      <c r="H40" s="95"/>
-      <c r="I40" s="94"/>
-      <c r="J40" s="94"/>
-      <c r="K40" s="94"/>
-      <c r="L40" s="94"/>
-      <c r="O40" s="121"/>
-      <c r="P40" s="111"/>
-      <c r="Q40" s="111"/>
-      <c r="R40" s="111"/>
-      <c r="S40" s="111"/>
-      <c r="T40" s="111"/>
-      <c r="U40" s="111"/>
-      <c r="V40" s="111"/>
-      <c r="W40" s="111"/>
-      <c r="X40" s="111"/>
-      <c r="Y40" s="111"/>
-      <c r="Z40" s="111"/>
-      <c r="AA40" s="116"/>
+      <c r="A40" s="96"/>
+      <c r="B40" s="97"/>
+      <c r="C40" s="99"/>
+      <c r="D40" s="99"/>
+      <c r="E40" s="99"/>
+      <c r="F40" s="124"/>
+      <c r="G40" s="124"/>
+      <c r="H40" s="124"/>
+      <c r="I40" s="99"/>
+      <c r="J40" s="99"/>
+      <c r="K40" s="99"/>
+      <c r="L40" s="99"/>
+      <c r="O40" s="122"/>
+      <c r="P40" s="101"/>
+      <c r="Q40" s="101"/>
+      <c r="R40" s="101"/>
+      <c r="S40" s="101"/>
+      <c r="T40" s="101"/>
+      <c r="U40" s="101"/>
+      <c r="V40" s="101"/>
+      <c r="W40" s="101"/>
+      <c r="X40" s="101"/>
+      <c r="Y40" s="101"/>
+      <c r="Z40" s="101"/>
+      <c r="AA40" s="117"/>
     </row>
     <row r="41" spans="1:27">
       <c r="A41" s="27" t="s">
@@ -3194,22 +3152,22 @@
       <c r="AA44" s="78"/>
     </row>
     <row r="45" spans="1:27" ht="57.75" customHeight="1" thickTop="1">
-      <c r="A45" s="91" t="s">
+      <c r="A45" s="126" t="s">
         <v>101</v>
       </c>
-      <c r="B45" s="92"/>
-      <c r="C45" s="92"/>
-      <c r="D45" s="92"/>
-      <c r="E45" s="92"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="92"/>
-      <c r="H45" s="92"/>
-      <c r="I45" s="101" t="s">
+      <c r="B45" s="127"/>
+      <c r="C45" s="127"/>
+      <c r="D45" s="127"/>
+      <c r="E45" s="127"/>
+      <c r="F45" s="127"/>
+      <c r="G45" s="127"/>
+      <c r="H45" s="127"/>
+      <c r="I45" s="125" t="s">
         <v>102</v>
       </c>
-      <c r="J45" s="101"/>
-      <c r="K45" s="101"/>
-      <c r="L45" s="101"/>
+      <c r="J45" s="125"/>
+      <c r="K45" s="125"/>
+      <c r="L45" s="125"/>
     </row>
     <row r="48" spans="1:27">
       <c r="A48" s="5" t="s">
@@ -3217,50 +3175,50 @@
       </c>
     </row>
     <row r="49" spans="1:20">
-      <c r="A49" s="135" t="s">
+      <c r="A49" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="136"/>
+      <c r="B49" s="105"/>
       <c r="C49" s="65"/>
       <c r="D49" s="4" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:20">
-      <c r="A50" s="137" t="s">
+      <c r="A50" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="138"/>
+      <c r="B50" s="107"/>
       <c r="C50" s="66"/>
       <c r="D50" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:20">
-      <c r="A51" s="137" t="s">
+      <c r="A51" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="138"/>
+      <c r="B51" s="107"/>
       <c r="C51" s="66"/>
       <c r="D51" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:20">
-      <c r="A52" s="135" t="s">
+      <c r="A52" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="136"/>
+      <c r="B52" s="105"/>
       <c r="C52" s="65"/>
       <c r="D52" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:20">
-      <c r="A53" s="137" t="s">
+      <c r="A53" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="138"/>
+      <c r="B53" s="107"/>
       <c r="C53" s="66"/>
       <c r="D53" s="4" t="s">
         <v>53</v>
@@ -3270,10 +3228,10 @@
       </c>
     </row>
     <row r="54" spans="1:20" ht="42.75" customHeight="1">
-      <c r="A54" s="135" t="s">
+      <c r="A54" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B54" s="136"/>
+      <c r="B54" s="105"/>
       <c r="C54" s="65"/>
       <c r="D54" s="4" t="s">
         <v>55</v>
@@ -3286,10 +3244,10 @@
       </c>
     </row>
     <row r="55" spans="1:20" ht="28.5" customHeight="1">
-      <c r="A55" s="135" t="s">
+      <c r="A55" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="B55" s="136"/>
+      <c r="B55" s="105"/>
       <c r="C55" s="65"/>
       <c r="D55" s="4" t="s">
         <v>55</v>
@@ -3302,60 +3260,60 @@
       </c>
     </row>
     <row r="56" spans="1:20">
-      <c r="A56" s="96" t="s">
+      <c r="A56" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="97"/>
+      <c r="B56" s="129"/>
       <c r="C56" s="80"/>
       <c r="D56" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:20">
-      <c r="A57" s="98" t="s">
+      <c r="A57" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="98"/>
+      <c r="B57" s="130"/>
       <c r="C57" s="80"/>
       <c r="D57" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:20">
-      <c r="A58" s="99" t="s">
+      <c r="A58" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="100"/>
+      <c r="B58" s="132"/>
       <c r="C58" s="81"/>
       <c r="D58" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:20">
-      <c r="A59" s="99" t="s">
+      <c r="A59" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="B59" s="100"/>
+      <c r="B59" s="132"/>
       <c r="C59" s="81"/>
       <c r="D59" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:20">
-      <c r="A60" s="129" t="s">
+      <c r="A60" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="B60" s="129"/>
+      <c r="B60" s="114"/>
       <c r="C60" s="81"/>
       <c r="D60" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:20">
-      <c r="A61" s="130" t="s">
+      <c r="A61" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="B61" s="130"/>
+      <c r="B61" s="108"/>
       <c r="C61" s="82"/>
       <c r="D61" s="4" t="s">
         <v>105</v>
@@ -3365,10 +3323,10 @@
       </c>
     </row>
     <row r="62" spans="1:20">
-      <c r="A62" s="131" t="s">
+      <c r="A62" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="B62" s="132"/>
+      <c r="B62" s="116"/>
       <c r="C62" s="82"/>
       <c r="D62" s="4" t="s">
         <v>55</v>
@@ -3378,10 +3336,10 @@
       </c>
     </row>
     <row r="63" spans="1:20">
-      <c r="A63" s="131" t="s">
+      <c r="A63" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="132"/>
+      <c r="B63" s="116"/>
       <c r="C63" s="82"/>
       <c r="D63" s="4" t="s">
         <v>55</v>
@@ -3391,40 +3349,40 @@
       </c>
     </row>
     <row r="64" spans="1:20">
-      <c r="A64" s="131" t="s">
+      <c r="A64" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="B64" s="132"/>
+      <c r="B64" s="116"/>
       <c r="C64" s="82"/>
       <c r="D64" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:11">
-      <c r="A65" s="131" t="s">
+      <c r="A65" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="132"/>
+      <c r="B65" s="116"/>
       <c r="C65" s="82"/>
       <c r="D65" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="130" t="s">
+      <c r="A66" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="B66" s="130"/>
+      <c r="B66" s="108"/>
       <c r="C66" s="82"/>
       <c r="D66" s="4" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67" s="130" t="s">
+      <c r="A67" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="B67" s="130"/>
+      <c r="B67" s="108"/>
       <c r="C67" s="82"/>
       <c r="D67" s="4" t="str">
         <f>D61</f>
@@ -3432,20 +3390,20 @@
       </c>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="130" t="s">
+      <c r="A68" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="B68" s="130"/>
+      <c r="B68" s="108"/>
       <c r="C68" s="82"/>
       <c r="D68" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:11">
-      <c r="A69" s="130" t="s">
+      <c r="A69" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="B69" s="130"/>
+      <c r="B69" s="108"/>
       <c r="C69" s="82"/>
       <c r="D69" s="4" t="s">
         <v>55</v>
@@ -3455,10 +3413,10 @@
       </c>
     </row>
     <row r="70" spans="1:11">
-      <c r="A70" s="130" t="s">
+      <c r="A70" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="B70" s="130"/>
+      <c r="B70" s="108"/>
       <c r="C70" s="82"/>
       <c r="D70" s="4" t="s">
         <v>55</v>
@@ -3468,10 +3426,10 @@
       </c>
     </row>
     <row r="71" spans="1:11">
-      <c r="A71" s="130" t="s">
+      <c r="A71" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="B71" s="130"/>
+      <c r="B71" s="108"/>
       <c r="C71" s="82"/>
       <c r="D71" s="4" t="s">
         <v>55</v>
@@ -3481,10 +3439,10 @@
       </c>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="130" t="s">
+      <c r="A72" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="B72" s="130"/>
+      <c r="B72" s="108"/>
       <c r="C72" s="82"/>
       <c r="D72" s="4" t="s">
         <v>55</v>
@@ -3494,10 +3452,10 @@
       </c>
     </row>
     <row r="73" spans="1:11">
-      <c r="A73" s="130" t="s">
+      <c r="A73" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="B73" s="130"/>
+      <c r="B73" s="108"/>
       <c r="C73" s="82"/>
       <c r="D73" s="4" t="s">
         <v>55</v>
@@ -3507,10 +3465,10 @@
       </c>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="130" t="s">
+      <c r="A74" s="108" t="s">
         <v>44</v>
       </c>
-      <c r="B74" s="130"/>
+      <c r="B74" s="108"/>
       <c r="C74" s="82"/>
       <c r="D74" s="4" t="s">
         <v>55</v>
@@ -3520,10 +3478,10 @@
       </c>
     </row>
     <row r="75" spans="1:11">
-      <c r="A75" s="130" t="s">
+      <c r="A75" s="108" t="s">
         <v>45</v>
       </c>
-      <c r="B75" s="130"/>
+      <c r="B75" s="108"/>
       <c r="C75" s="82"/>
       <c r="D75" s="4" t="s">
         <v>55</v>
@@ -3533,10 +3491,10 @@
       </c>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="130" t="s">
+      <c r="A76" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="B76" s="130"/>
+      <c r="B76" s="108"/>
       <c r="C76" s="82"/>
       <c r="D76" s="4" t="s">
         <v>55</v>
@@ -3546,10 +3504,10 @@
       </c>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="130" t="s">
+      <c r="A77" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="B77" s="130"/>
+      <c r="B77" s="108"/>
       <c r="C77" s="82"/>
       <c r="D77" s="4" t="s">
         <v>55</v>
@@ -3559,10 +3517,10 @@
       </c>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="130" t="s">
+      <c r="A78" s="108" t="s">
         <v>48</v>
       </c>
-      <c r="B78" s="130"/>
+      <c r="B78" s="108"/>
       <c r="C78" s="82"/>
       <c r="D78" s="4" t="s">
         <v>55</v>
@@ -3584,38 +3542,38 @@
       <c r="H81" s="22"/>
     </row>
     <row r="82" spans="1:33" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A82" s="113" t="s">
+      <c r="A82" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="B82" s="114"/>
-      <c r="C82" s="114"/>
-      <c r="D82" s="114"/>
-      <c r="E82" s="114"/>
-      <c r="F82" s="114"/>
-      <c r="G82" s="114"/>
-      <c r="H82" s="114"/>
-      <c r="I82" s="114"/>
-      <c r="J82" s="114"/>
-      <c r="K82" s="114"/>
-      <c r="L82" s="115"/>
-      <c r="O82" s="139" t="s">
+      <c r="B82" s="110"/>
+      <c r="C82" s="110"/>
+      <c r="D82" s="110"/>
+      <c r="E82" s="110"/>
+      <c r="F82" s="110"/>
+      <c r="G82" s="110"/>
+      <c r="H82" s="110"/>
+      <c r="I82" s="110"/>
+      <c r="J82" s="110"/>
+      <c r="K82" s="110"/>
+      <c r="L82" s="111"/>
+      <c r="O82" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="P82" s="140"/>
-      <c r="Q82" s="140"/>
-      <c r="R82" s="140"/>
-      <c r="S82" s="140"/>
-      <c r="T82" s="140"/>
-      <c r="U82" s="140"/>
-      <c r="V82" s="140"/>
-      <c r="W82" s="140"/>
-      <c r="X82" s="140"/>
-      <c r="Y82" s="140"/>
-      <c r="Z82" s="140"/>
-      <c r="AA82" s="140"/>
-      <c r="AB82" s="140"/>
-      <c r="AC82" s="140"/>
-      <c r="AD82" s="141"/>
+      <c r="P82" s="90"/>
+      <c r="Q82" s="90"/>
+      <c r="R82" s="90"/>
+      <c r="S82" s="90"/>
+      <c r="T82" s="90"/>
+      <c r="U82" s="90"/>
+      <c r="V82" s="90"/>
+      <c r="W82" s="90"/>
+      <c r="X82" s="90"/>
+      <c r="Y82" s="90"/>
+      <c r="Z82" s="90"/>
+      <c r="AA82" s="90"/>
+      <c r="AB82" s="90"/>
+      <c r="AC82" s="90"/>
+      <c r="AD82" s="91"/>
       <c r="AE82" s="79"/>
     </row>
     <row r="83" spans="1:33" ht="15" thickTop="1">
@@ -3692,17 +3650,17 @@
       <c r="AD85" s="52"/>
     </row>
     <row r="86" spans="1:33">
-      <c r="A86" s="123" t="s">
+      <c r="A86" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="B86" s="123"/>
-      <c r="C86" s="123"/>
-      <c r="D86" s="123"/>
-      <c r="E86" s="123"/>
-      <c r="F86" s="123"/>
-      <c r="G86" s="123"/>
-      <c r="H86" s="123"/>
-      <c r="I86" s="123"/>
+      <c r="B86" s="92"/>
+      <c r="C86" s="92"/>
+      <c r="D86" s="92"/>
+      <c r="E86" s="92"/>
+      <c r="F86" s="92"/>
+      <c r="G86" s="92"/>
+      <c r="H86" s="92"/>
+      <c r="I86" s="92"/>
       <c r="O86" s="51"/>
       <c r="P86" s="38"/>
       <c r="Q86" s="38"/>
@@ -3742,9 +3700,9 @@
       <c r="G87" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K87" s="124"/>
-      <c r="L87" s="125"/>
-      <c r="M87" s="125"/>
+      <c r="K87" s="93"/>
+      <c r="L87" s="94"/>
+      <c r="M87" s="94"/>
       <c r="O87" s="51"/>
       <c r="P87" s="38"/>
       <c r="Q87" s="38"/>
@@ -3858,31 +3816,31 @@
       <c r="AD90" s="52"/>
     </row>
     <row r="91" spans="1:33" ht="45" customHeight="1">
-      <c r="A91" s="126" t="s">
+      <c r="A91" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="128" t="s">
+      <c r="B91" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="C91" s="104" t="s">
+      <c r="C91" s="135" t="s">
         <v>125</v>
       </c>
-      <c r="D91" s="110" t="s">
+      <c r="D91" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="E91" s="93" t="s">
+      <c r="E91" s="98" t="s">
         <v>19</v>
       </c>
       <c r="F91" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="G91" s="93" t="s">
+      <c r="G91" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="H91" s="133" t="s">
+      <c r="H91" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="I91" s="93" t="s">
+      <c r="I91" s="98" t="s">
         <v>22</v>
       </c>
       <c r="J91" s="24" t="s">
@@ -3897,85 +3855,85 @@
       <c r="M91" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="O91" s="110" t="s">
+      <c r="O91" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="P91" s="111" t="s">
+      <c r="P91" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="Q91" s="111" t="s">
+      <c r="Q91" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="R91" s="111" t="s">
+      <c r="R91" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="S91" s="111" t="s">
+      <c r="S91" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="T91" s="111" t="s">
+      <c r="T91" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="U91" s="111" t="s">
+      <c r="U91" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="V91" s="111" t="s">
+      <c r="V91" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="W91" s="111" t="s">
+      <c r="W91" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="X91" s="111" t="s">
+      <c r="X91" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="Y91" s="111" t="s">
+      <c r="Y91" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="Z91" s="111" t="s">
+      <c r="Z91" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="AA91" s="111" t="s">
+      <c r="AA91" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="AB91" s="111" t="s">
+      <c r="AB91" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="AC91" s="111" t="s">
+      <c r="AC91" s="101" t="s">
         <v>74</v>
       </c>
-      <c r="AD91" s="112" t="s">
+      <c r="AD91" s="102" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="92" spans="1:33">
-      <c r="A92" s="127"/>
-      <c r="B92" s="128"/>
-      <c r="C92" s="105"/>
-      <c r="D92" s="110"/>
-      <c r="E92" s="94"/>
+      <c r="A92" s="96"/>
+      <c r="B92" s="97"/>
+      <c r="C92" s="136"/>
+      <c r="D92" s="100"/>
+      <c r="E92" s="99"/>
       <c r="F92" s="26"/>
-      <c r="G92" s="94"/>
-      <c r="H92" s="134"/>
-      <c r="I92" s="94"/>
+      <c r="G92" s="99"/>
+      <c r="H92" s="113"/>
+      <c r="I92" s="99"/>
       <c r="J92" s="26"/>
       <c r="K92" s="26"/>
       <c r="L92" s="26"/>
       <c r="M92" s="26"/>
-      <c r="O92" s="110"/>
-      <c r="P92" s="111"/>
-      <c r="Q92" s="111"/>
-      <c r="R92" s="111"/>
-      <c r="S92" s="111"/>
-      <c r="T92" s="111"/>
-      <c r="U92" s="111"/>
-      <c r="V92" s="111"/>
-      <c r="W92" s="111"/>
-      <c r="X92" s="111"/>
-      <c r="Y92" s="111"/>
-      <c r="Z92" s="111"/>
-      <c r="AA92" s="111"/>
-      <c r="AB92" s="111"/>
-      <c r="AC92" s="111"/>
-      <c r="AD92" s="112"/>
+      <c r="O92" s="100"/>
+      <c r="P92" s="101"/>
+      <c r="Q92" s="101"/>
+      <c r="R92" s="101"/>
+      <c r="S92" s="101"/>
+      <c r="T92" s="101"/>
+      <c r="U92" s="101"/>
+      <c r="V92" s="101"/>
+      <c r="W92" s="101"/>
+      <c r="X92" s="101"/>
+      <c r="Y92" s="101"/>
+      <c r="Z92" s="101"/>
+      <c r="AA92" s="101"/>
+      <c r="AB92" s="101"/>
+      <c r="AC92" s="101"/>
+      <c r="AD92" s="102"/>
     </row>
     <row r="93" spans="1:33" ht="15">
       <c r="A93" s="1" t="s">
@@ -4354,23 +4312,23 @@
       </c>
     </row>
     <row r="97" spans="1:31" ht="63" customHeight="1" thickTop="1">
-      <c r="A97" s="102" t="s">
+      <c r="A97" s="133" t="s">
         <v>101</v>
       </c>
-      <c r="B97" s="103"/>
-      <c r="C97" s="103"/>
-      <c r="D97" s="103"/>
-      <c r="E97" s="103"/>
-      <c r="F97" s="103"/>
-      <c r="G97" s="103"/>
-      <c r="H97" s="103"/>
-      <c r="I97" s="103"/>
-      <c r="J97" s="101" t="s">
+      <c r="B97" s="134"/>
+      <c r="C97" s="134"/>
+      <c r="D97" s="134"/>
+      <c r="E97" s="134"/>
+      <c r="F97" s="134"/>
+      <c r="G97" s="134"/>
+      <c r="H97" s="134"/>
+      <c r="I97" s="134"/>
+      <c r="J97" s="125" t="s">
         <v>102</v>
       </c>
-      <c r="K97" s="101"/>
-      <c r="L97" s="101"/>
-      <c r="M97" s="101"/>
+      <c r="K97" s="125"/>
+      <c r="L97" s="125"/>
+      <c r="M97" s="125"/>
     </row>
     <row r="98" spans="1:31" s="64" customFormat="1">
       <c r="A98" s="72"/>
@@ -4392,60 +4350,60 @@
       </c>
     </row>
     <row r="101" spans="1:31">
-      <c r="A101" s="111" t="s">
+      <c r="A101" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="B101" s="111"/>
+      <c r="B101" s="101"/>
       <c r="C101" s="83"/>
       <c r="D101" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="102" spans="1:31">
-      <c r="A102" s="111" t="s">
+      <c r="A102" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="B102" s="111"/>
+      <c r="B102" s="101"/>
       <c r="C102" s="83"/>
       <c r="D102" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="103" spans="1:31">
-      <c r="A103" s="111" t="s">
+      <c r="A103" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="B103" s="111"/>
+      <c r="B103" s="101"/>
       <c r="C103" s="83"/>
       <c r="D103" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:31">
-      <c r="A104" s="111" t="s">
+      <c r="A104" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="B104" s="111"/>
+      <c r="B104" s="101"/>
       <c r="C104" s="83"/>
       <c r="D104" s="4" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="105" spans="1:31">
-      <c r="A105" s="111" t="s">
+      <c r="A105" s="101" t="s">
         <v>74</v>
       </c>
-      <c r="B105" s="111"/>
+      <c r="B105" s="101"/>
       <c r="C105" s="83"/>
       <c r="D105" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:31">
-      <c r="A106" s="112" t="s">
+      <c r="A106" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="B106" s="112"/>
+      <c r="B106" s="102"/>
       <c r="C106" s="83"/>
       <c r="D106" s="4" t="s">
         <v>81</v>
@@ -4464,39 +4422,39 @@
       <c r="H110" s="22"/>
     </row>
     <row r="111" spans="1:31" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A111" s="113" t="s">
+      <c r="A111" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="B111" s="114"/>
-      <c r="C111" s="114"/>
-      <c r="D111" s="114"/>
-      <c r="E111" s="114"/>
-      <c r="F111" s="114"/>
-      <c r="G111" s="114"/>
-      <c r="H111" s="114"/>
-      <c r="I111" s="114"/>
-      <c r="J111" s="114"/>
-      <c r="K111" s="114"/>
-      <c r="L111" s="115"/>
-      <c r="O111" s="139" t="s">
+      <c r="B111" s="110"/>
+      <c r="C111" s="110"/>
+      <c r="D111" s="110"/>
+      <c r="E111" s="110"/>
+      <c r="F111" s="110"/>
+      <c r="G111" s="110"/>
+      <c r="H111" s="110"/>
+      <c r="I111" s="110"/>
+      <c r="J111" s="110"/>
+      <c r="K111" s="110"/>
+      <c r="L111" s="111"/>
+      <c r="O111" s="89" t="s">
         <v>87</v>
       </c>
-      <c r="P111" s="140"/>
-      <c r="Q111" s="140"/>
-      <c r="R111" s="140"/>
-      <c r="S111" s="140"/>
-      <c r="T111" s="140"/>
-      <c r="U111" s="140"/>
-      <c r="V111" s="140"/>
-      <c r="W111" s="140"/>
-      <c r="X111" s="140"/>
-      <c r="Y111" s="140"/>
-      <c r="Z111" s="140"/>
-      <c r="AA111" s="140"/>
-      <c r="AB111" s="140"/>
-      <c r="AC111" s="140"/>
-      <c r="AD111" s="140"/>
-      <c r="AE111" s="141"/>
+      <c r="P111" s="90"/>
+      <c r="Q111" s="90"/>
+      <c r="R111" s="90"/>
+      <c r="S111" s="90"/>
+      <c r="T111" s="90"/>
+      <c r="U111" s="90"/>
+      <c r="V111" s="90"/>
+      <c r="W111" s="90"/>
+      <c r="X111" s="90"/>
+      <c r="Y111" s="90"/>
+      <c r="Z111" s="90"/>
+      <c r="AA111" s="90"/>
+      <c r="AB111" s="90"/>
+      <c r="AC111" s="90"/>
+      <c r="AD111" s="90"/>
+      <c r="AE111" s="91"/>
     </row>
     <row r="112" spans="1:31" ht="15" thickTop="1">
       <c r="A112" s="5" t="s">
@@ -4575,17 +4533,17 @@
       <c r="AE114" s="52"/>
     </row>
     <row r="115" spans="1:34">
-      <c r="A115" s="123" t="s">
+      <c r="A115" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="B115" s="123"/>
-      <c r="C115" s="123"/>
-      <c r="D115" s="123"/>
-      <c r="E115" s="123"/>
-      <c r="F115" s="123"/>
-      <c r="G115" s="123"/>
-      <c r="H115" s="123"/>
-      <c r="I115" s="123"/>
+      <c r="B115" s="92"/>
+      <c r="C115" s="92"/>
+      <c r="D115" s="92"/>
+      <c r="E115" s="92"/>
+      <c r="F115" s="92"/>
+      <c r="G115" s="92"/>
+      <c r="H115" s="92"/>
+      <c r="I115" s="92"/>
       <c r="O115" s="51"/>
       <c r="P115" s="38"/>
       <c r="Q115" s="38"/>
@@ -4628,9 +4586,9 @@
       <c r="I116" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K116" s="124"/>
-      <c r="L116" s="125"/>
-      <c r="M116" s="125"/>
+      <c r="K116" s="93"/>
+      <c r="L116" s="94"/>
+      <c r="M116" s="94"/>
       <c r="O116" s="51"/>
       <c r="P116" s="38"/>
       <c r="Q116" s="38"/>
@@ -4750,28 +4708,28 @@
       <c r="AE119" s="52"/>
     </row>
     <row r="120" spans="1:34" ht="45" customHeight="1">
-      <c r="A120" s="126" t="s">
+      <c r="A120" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B120" s="128" t="s">
+      <c r="B120" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="C120" s="104" t="s">
+      <c r="C120" s="135" t="s">
         <v>123</v>
       </c>
-      <c r="D120" s="108" t="s">
+      <c r="D120" s="139" t="s">
         <v>37</v>
       </c>
-      <c r="E120" s="93" t="s">
+      <c r="E120" s="98" t="s">
         <v>122</v>
       </c>
       <c r="F120" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="G120" s="93" t="s">
+      <c r="G120" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="H120" s="106" t="s">
+      <c r="H120" s="137" t="s">
         <v>27</v>
       </c>
       <c r="I120" s="25" t="s">
@@ -4789,89 +4747,89 @@
       <c r="M120" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="O120" s="110" t="s">
+      <c r="O120" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="P120" s="111" t="s">
+      <c r="P120" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="Q120" s="111" t="s">
+      <c r="Q120" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="R120" s="111" t="s">
+      <c r="R120" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="S120" s="111" t="s">
+      <c r="S120" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="T120" s="111" t="s">
+      <c r="T120" s="101" t="s">
         <v>76</v>
       </c>
-      <c r="U120" s="111" t="s">
+      <c r="U120" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="V120" s="111" t="s">
+      <c r="V120" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="W120" s="111" t="s">
+      <c r="W120" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="X120" s="111" t="s">
+      <c r="X120" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="Y120" s="111" t="s">
+      <c r="Y120" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="Z120" s="111" t="s">
+      <c r="Z120" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="AA120" s="111" t="s">
+      <c r="AA120" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="AB120" s="111" t="s">
+      <c r="AB120" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="AC120" s="142" t="s">
+      <c r="AC120" s="103" t="s">
         <v>95</v>
       </c>
-      <c r="AD120" s="111" t="s">
+      <c r="AD120" s="101" t="s">
         <v>74</v>
       </c>
-      <c r="AE120" s="112" t="s">
+      <c r="AE120" s="102" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="121" spans="1:34">
-      <c r="A121" s="127"/>
-      <c r="B121" s="128"/>
-      <c r="C121" s="105"/>
-      <c r="D121" s="109"/>
-      <c r="E121" s="94"/>
+      <c r="A121" s="96"/>
+      <c r="B121" s="97"/>
+      <c r="C121" s="136"/>
+      <c r="D121" s="140"/>
+      <c r="E121" s="99"/>
       <c r="F121" s="26"/>
-      <c r="G121" s="94"/>
-      <c r="H121" s="107"/>
+      <c r="G121" s="99"/>
+      <c r="H121" s="138"/>
       <c r="I121" s="25"/>
       <c r="J121" s="26"/>
       <c r="K121" s="26"/>
       <c r="L121" s="26"/>
       <c r="M121" s="26"/>
-      <c r="O121" s="110"/>
-      <c r="P121" s="111"/>
-      <c r="Q121" s="111"/>
-      <c r="R121" s="111"/>
-      <c r="S121" s="111"/>
-      <c r="T121" s="111"/>
-      <c r="U121" s="111"/>
-      <c r="V121" s="111"/>
-      <c r="W121" s="111"/>
-      <c r="X121" s="111"/>
-      <c r="Y121" s="111"/>
-      <c r="Z121" s="111"/>
-      <c r="AA121" s="111"/>
-      <c r="AB121" s="111"/>
-      <c r="AC121" s="142"/>
-      <c r="AD121" s="111"/>
-      <c r="AE121" s="112"/>
+      <c r="O121" s="100"/>
+      <c r="P121" s="101"/>
+      <c r="Q121" s="101"/>
+      <c r="R121" s="101"/>
+      <c r="S121" s="101"/>
+      <c r="T121" s="101"/>
+      <c r="U121" s="101"/>
+      <c r="V121" s="101"/>
+      <c r="W121" s="101"/>
+      <c r="X121" s="101"/>
+      <c r="Y121" s="101"/>
+      <c r="Z121" s="101"/>
+      <c r="AA121" s="101"/>
+      <c r="AB121" s="101"/>
+      <c r="AC121" s="103"/>
+      <c r="AD121" s="101"/>
+      <c r="AE121" s="102"/>
     </row>
     <row r="122" spans="1:34" ht="15">
       <c r="A122" s="1" t="s">
@@ -5262,23 +5220,23 @@
       </c>
     </row>
     <row r="126" spans="1:34" ht="72" customHeight="1" thickTop="1">
-      <c r="A126" s="102" t="s">
+      <c r="A126" s="133" t="s">
         <v>101</v>
       </c>
-      <c r="B126" s="103"/>
-      <c r="C126" s="103"/>
-      <c r="D126" s="103"/>
-      <c r="E126" s="103"/>
-      <c r="F126" s="103"/>
-      <c r="G126" s="103"/>
-      <c r="H126" s="103"/>
-      <c r="I126" s="103"/>
-      <c r="J126" s="101" t="s">
+      <c r="B126" s="134"/>
+      <c r="C126" s="134"/>
+      <c r="D126" s="134"/>
+      <c r="E126" s="134"/>
+      <c r="F126" s="134"/>
+      <c r="G126" s="134"/>
+      <c r="H126" s="134"/>
+      <c r="I126" s="134"/>
+      <c r="J126" s="125" t="s">
         <v>102</v>
       </c>
-      <c r="K126" s="101"/>
-      <c r="L126" s="101"/>
-      <c r="M126" s="101"/>
+      <c r="K126" s="125"/>
+      <c r="L126" s="125"/>
+      <c r="M126" s="125"/>
       <c r="AC126" s="67" t="s">
         <v>124</v>
       </c>
@@ -5310,29 +5268,88 @@
     </row>
   </sheetData>
   <mergeCells count="129">
-    <mergeCell ref="O111:AE111"/>
-    <mergeCell ref="A115:I115"/>
-    <mergeCell ref="K116:M116"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="E120:E121"/>
-    <mergeCell ref="O120:O121"/>
-    <mergeCell ref="Y120:Y121"/>
-    <mergeCell ref="P120:P121"/>
-    <mergeCell ref="Q120:Q121"/>
-    <mergeCell ref="R120:R121"/>
-    <mergeCell ref="S120:S121"/>
-    <mergeCell ref="T120:T121"/>
-    <mergeCell ref="U120:U121"/>
-    <mergeCell ref="AB120:AB121"/>
-    <mergeCell ref="AD120:AD121"/>
-    <mergeCell ref="AE120:AE121"/>
-    <mergeCell ref="AC120:AC121"/>
-    <mergeCell ref="V120:V121"/>
-    <mergeCell ref="W120:W121"/>
-    <mergeCell ref="X120:X121"/>
-    <mergeCell ref="Z120:Z121"/>
-    <mergeCell ref="AA120:AA121"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="J126:M126"/>
+    <mergeCell ref="A126:I126"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="A97:I97"/>
+    <mergeCell ref="J97:M97"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="G120:G121"/>
+    <mergeCell ref="H120:H121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A111:L111"/>
+    <mergeCell ref="I45:L45"/>
+    <mergeCell ref="W39:W40"/>
+    <mergeCell ref="Y39:Y40"/>
+    <mergeCell ref="X39:X40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="Z39:Z40"/>
+    <mergeCell ref="U39:U40"/>
+    <mergeCell ref="V39:V40"/>
+    <mergeCell ref="AA39:AA40"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="O30:AA30"/>
+    <mergeCell ref="Q39:Q40"/>
+    <mergeCell ref="O39:O40"/>
+    <mergeCell ref="P39:P40"/>
+    <mergeCell ref="R39:R40"/>
+    <mergeCell ref="S39:S40"/>
+    <mergeCell ref="T39:T40"/>
+    <mergeCell ref="A10:J11"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="Z91:Z92"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A82:L82"/>
+    <mergeCell ref="A86:I86"/>
+    <mergeCell ref="K87:M87"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="H91:H92"/>
+    <mergeCell ref="I91:I92"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
     <mergeCell ref="AD91:AD92"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A50:B50"/>
@@ -5357,88 +5374,29 @@
     <mergeCell ref="P91:P92"/>
     <mergeCell ref="Q91:Q92"/>
     <mergeCell ref="Y91:Y92"/>
-    <mergeCell ref="Z91:Z92"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A82:L82"/>
-    <mergeCell ref="A86:I86"/>
-    <mergeCell ref="K87:M87"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="H91:H92"/>
-    <mergeCell ref="I91:I92"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="AA39:AA40"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="O30:AA30"/>
-    <mergeCell ref="Q39:Q40"/>
-    <mergeCell ref="O39:O40"/>
-    <mergeCell ref="P39:P40"/>
-    <mergeCell ref="R39:R40"/>
-    <mergeCell ref="S39:S40"/>
-    <mergeCell ref="T39:T40"/>
-    <mergeCell ref="A10:J11"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="I45:L45"/>
-    <mergeCell ref="W39:W40"/>
-    <mergeCell ref="Y39:Y40"/>
-    <mergeCell ref="X39:X40"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="Z39:Z40"/>
-    <mergeCell ref="U39:U40"/>
-    <mergeCell ref="V39:V40"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="J126:M126"/>
-    <mergeCell ref="A126:I126"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="A97:I97"/>
-    <mergeCell ref="J97:M97"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="G120:G121"/>
-    <mergeCell ref="H120:H121"/>
-    <mergeCell ref="D120:D121"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A111:L111"/>
+    <mergeCell ref="O111:AE111"/>
+    <mergeCell ref="A115:I115"/>
+    <mergeCell ref="K116:M116"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="E120:E121"/>
+    <mergeCell ref="O120:O121"/>
+    <mergeCell ref="Y120:Y121"/>
+    <mergeCell ref="P120:P121"/>
+    <mergeCell ref="Q120:Q121"/>
+    <mergeCell ref="R120:R121"/>
+    <mergeCell ref="S120:S121"/>
+    <mergeCell ref="T120:T121"/>
+    <mergeCell ref="U120:U121"/>
+    <mergeCell ref="AB120:AB121"/>
+    <mergeCell ref="AD120:AD121"/>
+    <mergeCell ref="AE120:AE121"/>
+    <mergeCell ref="AC120:AC121"/>
+    <mergeCell ref="V120:V121"/>
+    <mergeCell ref="W120:W121"/>
+    <mergeCell ref="X120:X121"/>
+    <mergeCell ref="Z120:Z121"/>
+    <mergeCell ref="AA120:AA121"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5449,17 +5407,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="90" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="144" customWidth="1"/>
     <col min="5" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="90" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="144" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5473,7 +5431,7 @@
       <c r="C1" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="141" t="s">
         <v>37</v>
       </c>
       <c r="E1" s="87" t="s">
@@ -5485,7 +5443,7 @@
       <c r="G1" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="88" t="s">
+      <c r="H1" s="141" t="s">
         <v>27</v>
       </c>
       <c r="I1" s="87" t="s">
@@ -5502,7 +5460,7 @@
       <c r="C2" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="89">
+      <c r="D2" s="142">
         <v>42229</v>
       </c>
       <c r="E2" s="86">
@@ -5514,7 +5472,7 @@
       <c r="G2" s="86">
         <v>2385</v>
       </c>
-      <c r="H2" s="89">
+      <c r="H2" s="142">
         <v>42234</v>
       </c>
       <c r="I2" s="86">
@@ -5534,7 +5492,7 @@
       <c r="C3" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="89">
+      <c r="D3" s="142">
         <v>42195</v>
       </c>
       <c r="E3" s="86">
@@ -5546,7 +5504,7 @@
       <c r="G3" s="86">
         <v>1885</v>
       </c>
-      <c r="H3" s="89">
+      <c r="H3" s="142">
         <v>42231</v>
       </c>
       <c r="I3" s="86">
@@ -5566,7 +5524,7 @@
       <c r="C4" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="89">
+      <c r="D4" s="142">
         <v>42235</v>
       </c>
       <c r="E4" s="86">
@@ -5578,7 +5536,7 @@
       <c r="G4" s="86">
         <v>826</v>
       </c>
-      <c r="H4" s="89">
+      <c r="H4" s="142">
         <v>42242</v>
       </c>
       <c r="I4" s="86">
@@ -5598,7 +5556,7 @@
       <c r="C5" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="89">
+      <c r="D5" s="142">
         <v>42197</v>
       </c>
       <c r="E5" s="86">
@@ -5610,7 +5568,7 @@
       <c r="G5" s="86">
         <v>292</v>
       </c>
-      <c r="H5" s="89">
+      <c r="H5" s="142">
         <v>42216</v>
       </c>
       <c r="I5" s="86">
@@ -5630,7 +5588,7 @@
       <c r="C6" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="89">
+      <c r="D6" s="142">
         <v>42373</v>
       </c>
       <c r="E6" s="86">
@@ -5643,8 +5601,8 @@
         <f>E6*95%</f>
         <v>133.85499999999999</v>
       </c>
-      <c r="H6" s="89">
-        <v>42373</v>
+      <c r="H6" s="142">
+        <v>42375</v>
       </c>
       <c r="I6" s="86">
         <v>140.9</v>
@@ -5663,7 +5621,7 @@
       <c r="C7" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="89">
+      <c r="D7" s="142">
         <v>42373</v>
       </c>
       <c r="E7" s="86">
@@ -5676,7 +5634,7 @@
         <f t="shared" ref="G7:G33" si="0">E7*95%</f>
         <v>135.28</v>
       </c>
-      <c r="H7" s="89">
+      <c r="H7" s="142">
         <v>42373</v>
       </c>
       <c r="I7" s="86">
@@ -5693,7 +5651,7 @@
       <c r="C8" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="89">
+      <c r="D8" s="142">
         <v>42374</v>
       </c>
       <c r="E8" s="86">
@@ -5706,7 +5664,7 @@
         <f t="shared" si="0"/>
         <v>248.71</v>
       </c>
-      <c r="H8" s="89">
+      <c r="H8" s="142">
         <v>42374</v>
       </c>
       <c r="I8" s="86">
@@ -5723,7 +5681,7 @@
       <c r="C9" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="89">
+      <c r="D9" s="142">
         <v>42375</v>
       </c>
       <c r="E9" s="86">
@@ -5736,7 +5694,7 @@
         <f t="shared" si="0"/>
         <v>310.64999999999998</v>
       </c>
-      <c r="H9" s="89">
+      <c r="H9" s="142">
         <v>42375</v>
       </c>
       <c r="I9" s="86">
@@ -5753,7 +5711,7 @@
       <c r="C10" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="89">
+      <c r="D10" s="142">
         <v>42376</v>
       </c>
       <c r="E10" s="86">
@@ -5766,7 +5724,7 @@
         <f t="shared" si="0"/>
         <v>307.13499999999999</v>
       </c>
-      <c r="H10" s="89">
+      <c r="H10" s="142">
         <v>42376</v>
       </c>
       <c r="I10" s="86">
@@ -5783,7 +5741,7 @@
       <c r="C11" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="89">
+      <c r="D11" s="142">
         <v>42377</v>
       </c>
       <c r="E11" s="86">
@@ -5796,7 +5754,7 @@
         <f t="shared" si="0"/>
         <v>333.92500000000001</v>
       </c>
-      <c r="H11" s="89">
+      <c r="H11" s="142">
         <v>42377</v>
       </c>
       <c r="I11" s="86">
@@ -5813,7 +5771,7 @@
       <c r="C12" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="89">
+      <c r="D12" s="142">
         <v>42380</v>
       </c>
       <c r="E12" s="86">
@@ -5826,7 +5784,7 @@
         <f t="shared" si="0"/>
         <v>194.56</v>
       </c>
-      <c r="H12" s="89">
+      <c r="H12" s="142">
         <v>42380</v>
       </c>
       <c r="I12" s="86">
@@ -5843,7 +5801,7 @@
       <c r="C13" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="89">
+      <c r="D13" s="142">
         <v>42380</v>
       </c>
       <c r="E13" s="86">
@@ -5856,7 +5814,7 @@
         <f t="shared" si="0"/>
         <v>299.82</v>
       </c>
-      <c r="H13" s="89">
+      <c r="H13" s="142">
         <v>42380</v>
       </c>
       <c r="I13" s="86">
@@ -5873,7 +5831,7 @@
       <c r="C14" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="89">
+      <c r="D14" s="142">
         <v>42381</v>
       </c>
       <c r="E14" s="86">
@@ -5886,7 +5844,7 @@
         <f t="shared" si="0"/>
         <v>1281.55</v>
       </c>
-      <c r="H14" s="89">
+      <c r="H14" s="142">
         <v>42381</v>
       </c>
       <c r="I14" s="86">
@@ -5903,7 +5861,7 @@
       <c r="C15" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="89">
+      <c r="D15" s="142">
         <v>42381</v>
       </c>
       <c r="E15" s="86">
@@ -5916,7 +5874,7 @@
         <f t="shared" si="0"/>
         <v>132.52500000000001</v>
       </c>
-      <c r="H15" s="89">
+      <c r="H15" s="142">
         <v>42381</v>
       </c>
       <c r="I15" s="86">
@@ -5936,7 +5894,7 @@
       <c r="C16" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="89">
+      <c r="D16" s="142">
         <v>42382</v>
       </c>
       <c r="E16" s="86">
@@ -5949,7 +5907,7 @@
         <f t="shared" si="0"/>
         <v>852.15</v>
       </c>
-      <c r="H16" s="89">
+      <c r="H16" s="142">
         <v>42382</v>
       </c>
       <c r="I16" s="86">
@@ -5966,7 +5924,7 @@
       <c r="C17" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="89">
+      <c r="D17" s="142">
         <v>42382</v>
       </c>
       <c r="E17" s="86">
@@ -5979,7 +5937,7 @@
         <f t="shared" si="0"/>
         <v>247</v>
       </c>
-      <c r="H17" s="89">
+      <c r="H17" s="142">
         <v>42382</v>
       </c>
       <c r="I17" s="86">
@@ -5996,7 +5954,7 @@
       <c r="C18" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="89">
+      <c r="D18" s="142">
         <v>42383</v>
       </c>
       <c r="E18" s="86">
@@ -6009,7 +5967,7 @@
         <f t="shared" si="0"/>
         <v>516.13499999999988</v>
       </c>
-      <c r="H18" s="89">
+      <c r="H18" s="142">
         <v>42383</v>
       </c>
       <c r="I18" s="86">
@@ -6026,7 +5984,7 @@
       <c r="C19" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="89">
+      <c r="D19" s="142">
         <v>42384</v>
       </c>
       <c r="E19" s="86">
@@ -6039,7 +5997,7 @@
         <f t="shared" si="0"/>
         <v>115.23499999999999</v>
       </c>
-      <c r="H19" s="89">
+      <c r="H19" s="142">
         <v>42384</v>
       </c>
       <c r="I19" s="86">
@@ -6056,7 +6014,7 @@
       <c r="C20" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="89">
+      <c r="D20" s="142">
         <v>42384</v>
       </c>
       <c r="E20" s="86">
@@ -6069,7 +6027,7 @@
         <f t="shared" si="0"/>
         <v>875.66249999999991</v>
       </c>
-      <c r="H20" s="89">
+      <c r="H20" s="142">
         <v>42384</v>
       </c>
       <c r="I20" s="86">
@@ -6086,7 +6044,7 @@
       <c r="C21" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="89">
+      <c r="D21" s="142">
         <v>42387</v>
       </c>
       <c r="E21" s="86">
@@ -6099,7 +6057,7 @@
         <f t="shared" si="0"/>
         <v>301.52999999999997</v>
       </c>
-      <c r="H21" s="89">
+      <c r="H21" s="142">
         <v>42387</v>
       </c>
       <c r="I21" s="86">
@@ -6116,7 +6074,7 @@
       <c r="C22" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="89">
+      <c r="D22" s="142">
         <v>42387</v>
       </c>
       <c r="E22" s="86">
@@ -6129,7 +6087,7 @@
         <f t="shared" si="0"/>
         <v>211.85</v>
       </c>
-      <c r="H22" s="89">
+      <c r="H22" s="142">
         <v>42387</v>
       </c>
       <c r="I22" s="86">
@@ -6146,7 +6104,7 @@
       <c r="C23" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="89">
+      <c r="D23" s="142">
         <v>42388</v>
       </c>
       <c r="E23" s="86">
@@ -6159,7 +6117,7 @@
         <f t="shared" si="0"/>
         <v>362.14</v>
       </c>
-      <c r="H23" s="89">
+      <c r="H23" s="142">
         <v>42388</v>
       </c>
       <c r="I23" s="86">
@@ -6176,7 +6134,7 @@
       <c r="C24" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="89">
+      <c r="D24" s="142">
         <v>42389</v>
       </c>
       <c r="E24" s="86">
@@ -6189,7 +6147,7 @@
         <f>E24*105%</f>
         <v>400.15500000000003</v>
       </c>
-      <c r="H24" s="89">
+      <c r="H24" s="142">
         <v>42389</v>
       </c>
       <c r="I24" s="86">
@@ -6206,7 +6164,7 @@
       <c r="C25" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="89">
+      <c r="D25" s="142">
         <v>42389</v>
       </c>
       <c r="E25" s="86">
@@ -6219,7 +6177,7 @@
         <f t="shared" si="0"/>
         <v>806.07499999999993</v>
       </c>
-      <c r="H25" s="89">
+      <c r="H25" s="142">
         <v>42389</v>
       </c>
       <c r="I25" s="86">
@@ -6236,7 +6194,7 @@
       <c r="C26" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="89">
+      <c r="D26" s="142">
         <v>42390</v>
       </c>
       <c r="E26" s="86">
@@ -6249,7 +6207,7 @@
         <f t="shared" si="0"/>
         <v>372.4</v>
       </c>
-      <c r="H26" s="89">
+      <c r="H26" s="142">
         <v>42390</v>
       </c>
       <c r="I26" s="86">
@@ -6266,7 +6224,7 @@
       <c r="C27" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="89">
+      <c r="D27" s="142">
         <v>42391</v>
       </c>
       <c r="E27" s="86">
@@ -6279,7 +6237,7 @@
         <f t="shared" si="0"/>
         <v>953.04</v>
       </c>
-      <c r="H27" s="89">
+      <c r="H27" s="142">
         <v>42391</v>
       </c>
       <c r="I27" s="86">
@@ -6296,7 +6254,7 @@
       <c r="C28" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="89">
+      <c r="D28" s="142">
         <v>42396</v>
       </c>
       <c r="E28" s="86">
@@ -6309,7 +6267,7 @@
         <f t="shared" si="0"/>
         <v>779.94999999999993</v>
       </c>
-      <c r="H28" s="89">
+      <c r="H28" s="142">
         <v>42396</v>
       </c>
       <c r="I28" s="86">
@@ -6326,7 +6284,7 @@
       <c r="C29" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="89">
+      <c r="D29" s="142">
         <v>42397</v>
       </c>
       <c r="E29" s="86">
@@ -6339,7 +6297,7 @@
         <f t="shared" si="0"/>
         <v>990.61249999999995</v>
       </c>
-      <c r="H29" s="89">
+      <c r="H29" s="142">
         <v>42397</v>
       </c>
       <c r="I29" s="86">
@@ -6356,7 +6314,7 @@
       <c r="C30" s="86" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="89">
+      <c r="D30" s="142">
         <v>42398</v>
       </c>
       <c r="E30" s="86">
@@ -6369,310 +6327,310 @@
         <f t="shared" si="0"/>
         <v>1092.2149999999999</v>
       </c>
-      <c r="H30" s="89">
+      <c r="H30" s="142">
         <v>42398</v>
       </c>
       <c r="I30" s="86">
         <v>1155</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="143" customFormat="1">
-      <c r="A31" s="143" t="s">
+    <row r="31" spans="1:9" s="88" customFormat="1">
+      <c r="A31" s="88" t="s">
         <v>335</v>
       </c>
-      <c r="B31" s="143" t="s">
+      <c r="B31" s="88" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="144">
+      <c r="C31" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="143">
         <v>42387</v>
       </c>
-      <c r="E31" s="143">
+      <c r="E31" s="88">
         <v>317.39999999999998</v>
       </c>
-      <c r="F31" s="143">
+      <c r="F31" s="88">
         <v>314.39999999999998</v>
       </c>
-      <c r="G31" s="143">
+      <c r="G31" s="88">
         <f t="shared" si="0"/>
         <v>301.52999999999997</v>
       </c>
-      <c r="H31" s="144">
+      <c r="H31" s="143">
         <v>42387</v>
       </c>
-      <c r="I31" s="143">
+      <c r="I31" s="88">
         <v>314.39999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="143" customFormat="1">
-      <c r="A32" s="143" t="s">
+    <row r="32" spans="1:9" s="88" customFormat="1">
+      <c r="A32" s="88" t="s">
         <v>336</v>
       </c>
-      <c r="B32" s="143" t="s">
+      <c r="B32" s="88" t="s">
         <v>138</v>
       </c>
-      <c r="C32" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="144">
+      <c r="C32" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="143">
         <v>42387</v>
       </c>
-      <c r="E32" s="143">
+      <c r="E32" s="88">
         <v>223</v>
       </c>
-      <c r="F32" s="143">
+      <c r="F32" s="88">
         <v>224.1</v>
       </c>
-      <c r="G32" s="143">
+      <c r="G32" s="88">
         <f t="shared" si="0"/>
         <v>211.85</v>
       </c>
-      <c r="H32" s="144">
+      <c r="H32" s="143">
         <v>42387</v>
       </c>
-      <c r="I32" s="143">
+      <c r="I32" s="88">
         <v>224.1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="143" customFormat="1">
-      <c r="A33" s="143" t="s">
+    <row r="33" spans="1:9" s="88" customFormat="1">
+      <c r="A33" s="88" t="s">
         <v>337</v>
       </c>
-      <c r="B33" s="143" t="s">
+      <c r="B33" s="88" t="s">
         <v>139</v>
       </c>
-      <c r="C33" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="144">
+      <c r="C33" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="143">
         <v>42388</v>
       </c>
-      <c r="E33" s="143">
+      <c r="E33" s="88">
         <v>381.2</v>
       </c>
-      <c r="F33" s="143">
+      <c r="F33" s="88">
         <v>388</v>
       </c>
-      <c r="G33" s="143">
+      <c r="G33" s="88">
         <f t="shared" si="0"/>
         <v>362.14</v>
       </c>
-      <c r="H33" s="144">
+      <c r="H33" s="143">
         <v>42388</v>
       </c>
-      <c r="I33" s="143">
+      <c r="I33" s="88">
         <v>388</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="143" customFormat="1">
-      <c r="A34" s="143" t="s">
+    <row r="34" spans="1:9" s="88" customFormat="1">
+      <c r="A34" s="88" t="s">
         <v>338</v>
       </c>
-      <c r="B34" s="143" t="s">
+      <c r="B34" s="88" t="s">
         <v>139</v>
       </c>
-      <c r="C34" s="143" t="s">
+      <c r="C34" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="144">
+      <c r="D34" s="143">
         <v>42389</v>
       </c>
-      <c r="E34" s="143">
+      <c r="E34" s="88">
         <v>381.1</v>
       </c>
-      <c r="F34" s="143">
+      <c r="F34" s="88">
         <v>376.5</v>
       </c>
-      <c r="G34" s="143">
+      <c r="G34" s="88">
         <f>E34*105%</f>
         <v>400.15500000000003</v>
       </c>
-      <c r="H34" s="144">
+      <c r="H34" s="143">
         <v>42389</v>
       </c>
-      <c r="I34" s="143">
+      <c r="I34" s="88">
         <v>385.70000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="143" customFormat="1">
-      <c r="A35" s="143" t="s">
+    <row r="35" spans="1:9" s="88" customFormat="1">
+      <c r="A35" s="88" t="s">
         <v>339</v>
       </c>
-      <c r="B35" s="143" t="s">
+      <c r="B35" s="88" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="144">
+      <c r="C35" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="143">
         <v>42389</v>
       </c>
-      <c r="E35" s="143">
+      <c r="E35" s="88">
         <v>848.5</v>
       </c>
-      <c r="F35" s="143">
+      <c r="F35" s="88">
         <v>834.1</v>
       </c>
-      <c r="G35" s="143">
+      <c r="G35" s="88">
         <f t="shared" ref="G35:G40" si="1">E35*95%</f>
         <v>806.07499999999993</v>
       </c>
-      <c r="H35" s="144">
+      <c r="H35" s="143">
         <v>42389</v>
       </c>
-      <c r="I35" s="143">
+      <c r="I35" s="88">
         <v>834.1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="143" customFormat="1">
-      <c r="A36" s="143" t="s">
+    <row r="36" spans="1:9" s="88" customFormat="1">
+      <c r="A36" s="88" t="s">
         <v>340</v>
       </c>
-      <c r="B36" s="143" t="s">
+      <c r="B36" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="C36" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="144">
+      <c r="C36" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="143">
         <v>42390</v>
       </c>
-      <c r="E36" s="143">
+      <c r="E36" s="88">
         <v>392</v>
       </c>
-      <c r="F36" s="143">
+      <c r="F36" s="88">
         <v>386.5</v>
       </c>
-      <c r="G36" s="143">
+      <c r="G36" s="88">
         <f t="shared" si="1"/>
         <v>372.4</v>
       </c>
-      <c r="H36" s="144">
+      <c r="H36" s="143">
         <v>42390</v>
       </c>
-      <c r="I36" s="143">
+      <c r="I36" s="88">
         <v>386.5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="143" customFormat="1">
-      <c r="A37" s="143" t="s">
+    <row r="37" spans="1:9" s="88" customFormat="1">
+      <c r="A37" s="88" t="s">
         <v>341</v>
       </c>
-      <c r="B37" s="143" t="s">
+      <c r="B37" s="88" t="s">
         <v>142</v>
       </c>
-      <c r="C37" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" s="144">
+      <c r="C37" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="143">
         <v>42391</v>
       </c>
-      <c r="E37" s="143">
+      <c r="E37" s="88">
         <v>1003.2</v>
       </c>
-      <c r="F37" s="143">
+      <c r="F37" s="88">
         <v>1010.5</v>
       </c>
-      <c r="G37" s="143">
+      <c r="G37" s="88">
         <f t="shared" si="1"/>
         <v>953.04</v>
       </c>
-      <c r="H37" s="144">
+      <c r="H37" s="143">
         <v>42391</v>
       </c>
-      <c r="I37" s="143">
+      <c r="I37" s="88">
         <v>1010.5</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="143" customFormat="1">
-      <c r="A38" s="143" t="s">
+    <row r="38" spans="1:9" s="88" customFormat="1">
+      <c r="A38" s="88" t="s">
         <v>342</v>
       </c>
-      <c r="B38" s="143" t="s">
+      <c r="B38" s="88" t="s">
         <v>143</v>
       </c>
-      <c r="C38" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="144">
+      <c r="C38" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="143">
         <v>42396</v>
       </c>
-      <c r="E38" s="143">
+      <c r="E38" s="88">
         <v>821</v>
       </c>
-      <c r="F38" s="143">
+      <c r="F38" s="88">
         <v>813.5</v>
       </c>
-      <c r="G38" s="143">
+      <c r="G38" s="88">
         <f t="shared" si="1"/>
         <v>779.94999999999993</v>
       </c>
-      <c r="H38" s="144">
+      <c r="H38" s="143">
         <v>42396</v>
       </c>
-      <c r="I38" s="143">
+      <c r="I38" s="88">
         <v>813.5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="143" customFormat="1">
-      <c r="A39" s="143" t="s">
+    <row r="39" spans="1:9" s="88" customFormat="1">
+      <c r="A39" s="88" t="s">
         <v>343</v>
       </c>
-      <c r="B39" s="143" t="s">
+      <c r="B39" s="88" t="s">
         <v>144</v>
       </c>
-      <c r="C39" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="144">
+      <c r="C39" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="143">
         <v>42397</v>
       </c>
-      <c r="E39" s="143">
+      <c r="E39" s="88">
         <v>1042.75</v>
       </c>
-      <c r="F39" s="143">
+      <c r="F39" s="88">
         <v>1046.5</v>
       </c>
-      <c r="G39" s="143">
+      <c r="G39" s="88">
         <f t="shared" si="1"/>
         <v>990.61249999999995</v>
       </c>
-      <c r="H39" s="144">
+      <c r="H39" s="143">
         <v>42397</v>
       </c>
-      <c r="I39" s="143">
+      <c r="I39" s="88">
         <v>1046.5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="143" customFormat="1">
-      <c r="A40" s="143" t="s">
+    <row r="40" spans="1:9" s="88" customFormat="1">
+      <c r="A40" s="88" t="s">
         <v>344</v>
       </c>
-      <c r="B40" s="143" t="s">
+      <c r="B40" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="C40" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="144">
+      <c r="C40" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="143">
         <v>42398</v>
       </c>
-      <c r="E40" s="143">
+      <c r="E40" s="88">
         <v>1149.7</v>
       </c>
-      <c r="F40" s="143">
+      <c r="F40" s="88">
         <v>1155</v>
       </c>
-      <c r="G40" s="143">
+      <c r="G40" s="88">
         <f t="shared" si="1"/>
         <v>1092.2149999999999</v>
       </c>
-      <c r="H40" s="144">
+      <c r="H40" s="143">
         <v>42398</v>
       </c>
-      <c r="I40" s="143">
+      <c r="I40" s="88">
         <v>1155</v>
       </c>
     </row>

</xml_diff>